<commit_message>
Optimize LSTM model in lstm2.py by adjusting hyperparameters and early stopping criteria; remove redundant VCS mapping in .idea/vcs.xml; delete outdated predictions_values.xlsx
</commit_message>
<xml_diff>
--- a/predictions_values.xlsx
+++ b/predictions_values.xlsx
@@ -459,7 +459,7 @@
         <v>44187.95833333334</v>
       </c>
       <c r="B2" t="n">
-        <v>17.82386779785156</v>
+        <v>0.4715113043785095</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -470,7 +470,7 @@
         <v>44188</v>
       </c>
       <c r="B3" t="n">
-        <v>17.00941467285156</v>
+        <v>5.960402965545654</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
@@ -481,7 +481,7 @@
         <v>44188.04166666666</v>
       </c>
       <c r="B4" t="n">
-        <v>14.6283712387085</v>
+        <v>8.232192039489746</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
@@ -492,7 +492,7 @@
         <v>44188.08333333334</v>
       </c>
       <c r="B5" t="n">
-        <v>10.64601039886475</v>
+        <v>8.950148582458496</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -503,7 +503,7 @@
         <v>44188.125</v>
       </c>
       <c r="B6" t="n">
-        <v>6.020278453826904</v>
+        <v>8.446547508239746</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
@@ -514,7 +514,7 @@
         <v>44188.16666666666</v>
       </c>
       <c r="B7" t="n">
-        <v>1.936660170555115</v>
+        <v>7.410171031951904</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
@@ -525,7 +525,7 @@
         <v>44188.20833333334</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.4760594964027405</v>
+        <v>5.990310192108154</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
@@ -536,7 +536,7 @@
         <v>44188.25</v>
       </c>
       <c r="B9" t="n">
-        <v>23.79249572753906</v>
+        <v>52.08851623535156</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
@@ -547,7 +547,7 @@
         <v>44188.29166666666</v>
       </c>
       <c r="B10" t="n">
-        <v>468.2033081054688</v>
+        <v>532.8381958007812</v>
       </c>
       <c r="C10" t="n">
         <v>487.9646638052137</v>
@@ -558,7 +558,7 @@
         <v>44188.33333333334</v>
       </c>
       <c r="B11" t="n">
-        <v>907.8894653320312</v>
+        <v>857.5928344726562</v>
       </c>
       <c r="C11" t="n">
         <v>866.0910018716376</v>
@@ -569,7 +569,7 @@
         <v>44188.375</v>
       </c>
       <c r="B12" t="n">
-        <v>902.510009765625</v>
+        <v>795.5382080078125</v>
       </c>
       <c r="C12" t="n">
         <v>860.9225120980739</v>
@@ -580,7 +580,7 @@
         <v>44188.41666666666</v>
       </c>
       <c r="B13" t="n">
-        <v>1073.325805664062</v>
+        <v>951.3601684570312</v>
       </c>
       <c r="C13" t="n">
         <v>1039.958306545641</v>
@@ -591,7 +591,7 @@
         <v>44188.45833333334</v>
       </c>
       <c r="B14" t="n">
-        <v>1062.399291992188</v>
+        <v>900.95263671875</v>
       </c>
       <c r="C14" t="n">
         <v>986.9411548574913</v>
@@ -602,7 +602,7 @@
         <v>44188.5</v>
       </c>
       <c r="B15" t="n">
-        <v>760.49658203125</v>
+        <v>570.752197265625</v>
       </c>
       <c r="C15" t="n">
         <v>710.1568378673246</v>
@@ -613,7 +613,7 @@
         <v>44188.54166666666</v>
       </c>
       <c r="B16" t="n">
-        <v>401.9512329101562</v>
+        <v>238.3490142822266</v>
       </c>
       <c r="C16" t="n">
         <v>271.8924186670402</v>
@@ -624,7 +624,7 @@
         <v>44188.58333333334</v>
       </c>
       <c r="B17" t="n">
-        <v>34.23457336425781</v>
+        <v>-69.49711608886719</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
@@ -635,7 +635,7 @@
         <v>44188.625</v>
       </c>
       <c r="B18" t="n">
-        <v>11.7433614730835</v>
+        <v>15.563063621521</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
@@ -646,7 +646,7 @@
         <v>44188.66666666666</v>
       </c>
       <c r="B19" t="n">
-        <v>15.72315883636475</v>
+        <v>-18.55894470214844</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
@@ -657,7 +657,7 @@
         <v>44188.70833333334</v>
       </c>
       <c r="B20" t="n">
-        <v>15.02625942230225</v>
+        <v>8.567946434020996</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
@@ -668,7 +668,7 @@
         <v>44188.75</v>
       </c>
       <c r="B21" t="n">
-        <v>12.41139125823975</v>
+        <v>18.65272521972656</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
@@ -679,7 +679,7 @@
         <v>44188.79166666666</v>
       </c>
       <c r="B22" t="n">
-        <v>14.00074672698975</v>
+        <v>11.15553188323975</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
@@ -690,7 +690,7 @@
         <v>44188.83333333334</v>
       </c>
       <c r="B23" t="n">
-        <v>8.000624656677246</v>
+        <v>10.433180809021</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
@@ -701,7 +701,7 @@
         <v>44188.875</v>
       </c>
       <c r="B24" t="n">
-        <v>4.878066539764404</v>
+        <v>8.631972312927246</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
@@ -712,7 +712,7 @@
         <v>44188.91666666666</v>
       </c>
       <c r="B25" t="n">
-        <v>14.049880027771</v>
+        <v>-13.875168800354</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
@@ -723,7 +723,7 @@
         <v>44188.95833333334</v>
       </c>
       <c r="B26" t="n">
-        <v>13.18836879730225</v>
+        <v>-6.790817737579346</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
@@ -734,7 +734,7 @@
         <v>44189</v>
       </c>
       <c r="B27" t="n">
-        <v>12.54884243011475</v>
+        <v>0.5021509528160095</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
@@ -745,7 +745,7 @@
         <v>44189.04166666666</v>
       </c>
       <c r="B28" t="n">
-        <v>11.13075160980225</v>
+        <v>4.437636852264404</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
@@ -756,7 +756,7 @@
         <v>44189.08333333334</v>
       </c>
       <c r="B29" t="n">
-        <v>9.362502098083496</v>
+        <v>6.820388317108154</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
@@ -767,7 +767,7 @@
         <v>44189.125</v>
       </c>
       <c r="B30" t="n">
-        <v>7.121474742889404</v>
+        <v>7.820083141326904</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
@@ -778,7 +778,7 @@
         <v>44189.16666666666</v>
       </c>
       <c r="B31" t="n">
-        <v>4.929091930389404</v>
+        <v>7.784621715545654</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
@@ -789,7 +789,7 @@
         <v>44189.20833333334</v>
       </c>
       <c r="B32" t="n">
-        <v>4.329604625701904</v>
+        <v>7.139907360076904</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
@@ -800,7 +800,7 @@
         <v>44189.25</v>
       </c>
       <c r="B33" t="n">
-        <v>14.96852016448975</v>
+        <v>27.99110412597656</v>
       </c>
       <c r="C33" t="n">
         <v>0</v>
@@ -811,7 +811,7 @@
         <v>44189.29166666666</v>
       </c>
       <c r="B34" t="n">
-        <v>437.310791015625</v>
+        <v>535.089111328125</v>
       </c>
       <c r="C34" t="n">
         <v>484.9692186680274</v>
@@ -822,7 +822,7 @@
         <v>44189.33333333334</v>
       </c>
       <c r="B35" t="n">
-        <v>560.9258422851562</v>
+        <v>570.7850952148438</v>
       </c>
       <c r="C35" t="n">
         <v>480.2273186365771</v>
@@ -833,7 +833,7 @@
         <v>44189.375</v>
       </c>
       <c r="B36" t="n">
-        <v>233.9442901611328</v>
+        <v>202.1988677978516</v>
       </c>
       <c r="C36" t="n">
         <v>218.3536445356711</v>
@@ -844,7 +844,7 @@
         <v>44189.41666666666</v>
       </c>
       <c r="B37" t="n">
-        <v>438.1145935058594</v>
+        <v>428.1760559082031</v>
       </c>
       <c r="C37" t="n">
         <v>443.3223025270851</v>
@@ -855,7 +855,7 @@
         <v>44189.45833333334</v>
       </c>
       <c r="B38" t="n">
-        <v>459.3896179199219</v>
+        <v>397.8950805664062</v>
       </c>
       <c r="C38" t="n">
         <v>334.7348020655131</v>
@@ -866,7 +866,7 @@
         <v>44189.5</v>
       </c>
       <c r="B39" t="n">
-        <v>387.4388427734375</v>
+        <v>348.9732055664062</v>
       </c>
       <c r="C39" t="n">
         <v>305.7404108390116</v>
@@ -877,7 +877,7 @@
         <v>44189.54166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>320.0675659179688</v>
+        <v>264.6585693359375</v>
       </c>
       <c r="C40" t="n">
         <v>190.3695477178923</v>
@@ -888,7 +888,7 @@
         <v>44189.58333333334</v>
       </c>
       <c r="B41" t="n">
-        <v>70.00184631347656</v>
+        <v>80.55110168457031</v>
       </c>
       <c r="C41" t="n">
         <v>0</v>
@@ -899,7 +899,7 @@
         <v>44189.625</v>
       </c>
       <c r="B42" t="n">
-        <v>32.82374572753906</v>
+        <v>21.96711730957031</v>
       </c>
       <c r="C42" t="n">
         <v>0</v>
@@ -910,7 +910,7 @@
         <v>44189.66666666666</v>
       </c>
       <c r="B43" t="n">
-        <v>32.37861633300781</v>
+        <v>3.119704723358154</v>
       </c>
       <c r="C43" t="n">
         <v>0</v>
@@ -921,7 +921,7 @@
         <v>44189.70833333334</v>
       </c>
       <c r="B44" t="n">
-        <v>18.17823791503906</v>
+        <v>18.98280334472656</v>
       </c>
       <c r="C44" t="n">
         <v>0</v>
@@ -932,7 +932,7 @@
         <v>44189.75</v>
       </c>
       <c r="B45" t="n">
-        <v>9.360976219177246</v>
+        <v>16.55567932128906</v>
       </c>
       <c r="C45" t="n">
         <v>0</v>
@@ -943,7 +943,7 @@
         <v>44189.79166666666</v>
       </c>
       <c r="B46" t="n">
-        <v>-0.1204076483845711</v>
+        <v>14.01502895355225</v>
       </c>
       <c r="C46" t="n">
         <v>0</v>
@@ -954,7 +954,7 @@
         <v>44189.83333333334</v>
       </c>
       <c r="B47" t="n">
-        <v>-0.9571385979652405</v>
+        <v>11.24647426605225</v>
       </c>
       <c r="C47" t="n">
         <v>0</v>
@@ -965,7 +965,7 @@
         <v>44189.875</v>
       </c>
       <c r="B48" t="n">
-        <v>3.951735973358154</v>
+        <v>8.387831687927246</v>
       </c>
       <c r="C48" t="n">
         <v>0</v>
@@ -976,7 +976,7 @@
         <v>44189.91666666666</v>
       </c>
       <c r="B49" t="n">
-        <v>9.909621238708496</v>
+        <v>-11.74730014801025</v>
       </c>
       <c r="C49" t="n">
         <v>0</v>
@@ -987,7 +987,7 @@
         <v>44189.95833333334</v>
       </c>
       <c r="B50" t="n">
-        <v>9.785109519958496</v>
+        <v>-6.091537952423096</v>
       </c>
       <c r="C50" t="n">
         <v>0</v>
@@ -998,7 +998,7 @@
         <v>44190</v>
       </c>
       <c r="B51" t="n">
-        <v>9.454360008239746</v>
+        <v>0.4627832770347595</v>
       </c>
       <c r="C51" t="n">
         <v>0</v>
@@ -1009,7 +1009,7 @@
         <v>44190.04166666666</v>
       </c>
       <c r="B52" t="n">
-        <v>8.778151512145996</v>
+        <v>4.042678356170654</v>
       </c>
       <c r="C52" t="n">
         <v>0</v>
@@ -1020,7 +1020,7 @@
         <v>44190.08333333334</v>
       </c>
       <c r="B53" t="n">
-        <v>7.218703746795654</v>
+        <v>5.912063121795654</v>
       </c>
       <c r="C53" t="n">
         <v>0</v>
@@ -1031,7 +1031,7 @@
         <v>44190.125</v>
       </c>
       <c r="B54" t="n">
-        <v>4.606826305389404</v>
+        <v>6.687819957733154</v>
       </c>
       <c r="C54" t="n">
         <v>0</v>
@@ -1042,7 +1042,7 @@
         <v>44190.16666666666</v>
       </c>
       <c r="B55" t="n">
-        <v>2.457595348358154</v>
+        <v>6.640578746795654</v>
       </c>
       <c r="C55" t="n">
         <v>0</v>
@@ -1053,7 +1053,7 @@
         <v>44190.20833333334</v>
       </c>
       <c r="B56" t="n">
-        <v>5.146132946014404</v>
+        <v>6.023025035858154</v>
       </c>
       <c r="C56" t="n">
         <v>0</v>
@@ -1064,7 +1064,7 @@
         <v>44190.25</v>
       </c>
       <c r="B57" t="n">
-        <v>4.256057262420654</v>
+        <v>9.785475730895996</v>
       </c>
       <c r="C57" t="n">
         <v>0</v>
@@ -1075,7 +1075,7 @@
         <v>44190.29166666666</v>
       </c>
       <c r="B58" t="n">
-        <v>260.134033203125</v>
+        <v>397.5484313964844</v>
       </c>
       <c r="C58" t="n">
         <v>331.6400134666502</v>
@@ -1086,7 +1086,7 @@
         <v>44190.33333333334</v>
       </c>
       <c r="B59" t="n">
-        <v>820.7582397460938</v>
+        <v>821.5111694335938</v>
       </c>
       <c r="C59" t="n">
         <v>830.4339730276638</v>
@@ -1097,7 +1097,7 @@
         <v>44190.375</v>
       </c>
       <c r="B60" t="n">
-        <v>659.8612060546875</v>
+        <v>586.8828125</v>
       </c>
       <c r="C60" t="n">
         <v>591.8765616099316</v>
@@ -1108,7 +1108,7 @@
         <v>44190.41666666666</v>
       </c>
       <c r="B61" t="n">
-        <v>716.4031982421875</v>
+        <v>559.6607055664062</v>
       </c>
       <c r="C61" t="n">
         <v>669.6282631353695</v>
@@ -1119,7 +1119,7 @@
         <v>44190.45833333334</v>
       </c>
       <c r="B62" t="n">
-        <v>980.9591674804688</v>
+        <v>850.01806640625</v>
       </c>
       <c r="C62" t="n">
         <v>917.2356701615514</v>
@@ -1130,7 +1130,7 @@
         <v>44190.5</v>
       </c>
       <c r="B63" t="n">
-        <v>523.7625732421875</v>
+        <v>422.9310302734375</v>
       </c>
       <c r="C63" t="n">
         <v>476.6209040589433</v>
@@ -1141,7 +1141,7 @@
         <v>44190.54166666666</v>
       </c>
       <c r="B64" t="n">
-        <v>380.9219055175781</v>
+        <v>273.3912963867188</v>
       </c>
       <c r="C64" t="n">
         <v>295.9604197740768</v>
@@ -1152,7 +1152,7 @@
         <v>44190.58333333334</v>
       </c>
       <c r="B65" t="n">
-        <v>27.18855285644531</v>
+        <v>8.015151023864746</v>
       </c>
       <c r="C65" t="n">
         <v>0</v>
@@ -1163,7 +1163,7 @@
         <v>44190.625</v>
       </c>
       <c r="B66" t="n">
-        <v>16.20649719238281</v>
+        <v>16.09162902832031</v>
       </c>
       <c r="C66" t="n">
         <v>0</v>
@@ -1174,7 +1174,7 @@
         <v>44190.66666666666</v>
       </c>
       <c r="B67" t="n">
-        <v>24.40400695800781</v>
+        <v>-31.52629089355469</v>
       </c>
       <c r="C67" t="n">
         <v>0</v>
@@ -1185,7 +1185,7 @@
         <v>44190.70833333334</v>
       </c>
       <c r="B68" t="n">
-        <v>20.27192687988281</v>
+        <v>15.94776821136475</v>
       </c>
       <c r="C68" t="n">
         <v>0</v>
@@ -1196,7 +1196,7 @@
         <v>44190.75</v>
       </c>
       <c r="B69" t="n">
-        <v>11.12147426605225</v>
+        <v>20.08613586425781</v>
       </c>
       <c r="C69" t="n">
         <v>0</v>
@@ -1207,7 +1207,7 @@
         <v>44190.79166666666</v>
       </c>
       <c r="B70" t="n">
-        <v>12.8004903793335</v>
+        <v>14.930983543396</v>
       </c>
       <c r="C70" t="n">
         <v>0</v>
@@ -1218,7 +1218,7 @@
         <v>44190.83333333334</v>
       </c>
       <c r="B71" t="n">
-        <v>4.677016735076904</v>
+        <v>12.989821434021</v>
       </c>
       <c r="C71" t="n">
         <v>0</v>
@@ -1229,7 +1229,7 @@
         <v>44190.875</v>
       </c>
       <c r="B72" t="n">
-        <v>7.397231578826904</v>
+        <v>9.927504539489746</v>
       </c>
       <c r="C72" t="n">
         <v>0</v>
@@ -1240,7 +1240,7 @@
         <v>44190.91666666666</v>
       </c>
       <c r="B73" t="n">
-        <v>8.617690086364746</v>
+        <v>-13.15757846832275</v>
       </c>
       <c r="C73" t="n">
         <v>0</v>
@@ -1251,7 +1251,7 @@
         <v>44190.95833333334</v>
       </c>
       <c r="B74" t="n">
-        <v>9.621352195739746</v>
+        <v>-8.885117530822754</v>
       </c>
       <c r="C74" t="n">
         <v>0</v>
@@ -1262,7 +1262,7 @@
         <v>44191</v>
       </c>
       <c r="B75" t="n">
-        <v>9.729384422302246</v>
+        <v>-2.984299182891846</v>
       </c>
       <c r="C75" t="n">
         <v>0</v>
@@ -1273,7 +1273,7 @@
         <v>44191.04166666666</v>
       </c>
       <c r="B76" t="n">
-        <v>9.129652976989746</v>
+        <v>1.793227553367615</v>
       </c>
       <c r="C76" t="n">
         <v>0</v>
@@ -1284,7 +1284,7 @@
         <v>44191.08333333334</v>
       </c>
       <c r="B77" t="n">
-        <v>7.802199840545654</v>
+        <v>4.835830211639404</v>
       </c>
       <c r="C77" t="n">
         <v>0</v>
@@ -1295,7 +1295,7 @@
         <v>44191.125</v>
       </c>
       <c r="B78" t="n">
-        <v>5.740127086639404</v>
+        <v>6.724807262420654</v>
       </c>
       <c r="C78" t="n">
         <v>0</v>
@@ -1306,7 +1306,7 @@
         <v>44191.16666666666</v>
       </c>
       <c r="B79" t="n">
-        <v>6.945144176483154</v>
+        <v>7.526809215545654</v>
       </c>
       <c r="C79" t="n">
         <v>0</v>
@@ -1317,7 +1317,7 @@
         <v>44191.20833333334</v>
       </c>
       <c r="B80" t="n">
-        <v>5.943496227264404</v>
+        <v>7.592299938201904</v>
       </c>
       <c r="C80" t="n">
         <v>0</v>
@@ -1328,7 +1328,7 @@
         <v>44191.25</v>
       </c>
       <c r="B81" t="n">
-        <v>33.19197082519531</v>
+        <v>76.51972961425781</v>
       </c>
       <c r="C81" t="n">
         <v>0</v>
@@ -1339,7 +1339,7 @@
         <v>44191.29166666666</v>
       </c>
       <c r="B82" t="n">
-        <v>351.2680053710938</v>
+        <v>464.6829223632812</v>
       </c>
       <c r="C82" t="n">
         <v>420.1804204259739</v>
@@ -1350,7 +1350,7 @@
         <v>44191.33333333334</v>
       </c>
       <c r="B83" t="n">
-        <v>418.9867553710938</v>
+        <v>512.1543579101562</v>
       </c>
       <c r="C83" t="n">
         <v>423.8823937920365</v>
@@ -1361,7 +1361,7 @@
         <v>44191.375</v>
       </c>
       <c r="B84" t="n">
-        <v>651.5538330078125</v>
+        <v>636.1698608398438</v>
       </c>
       <c r="C84" t="n">
         <v>647.8101087358848</v>
@@ -1372,7 +1372,7 @@
         <v>44191.41666666666</v>
       </c>
       <c r="B85" t="n">
-        <v>656</v>
+        <v>542.3331298828125</v>
       </c>
       <c r="C85" t="n">
         <v>564.0148653228073</v>
@@ -1383,7 +1383,7 @@
         <v>44191.45833333334</v>
       </c>
       <c r="B86" t="n">
-        <v>817.43994140625</v>
+        <v>686.6143188476562</v>
       </c>
       <c r="C86" t="n">
         <v>718.749735073161</v>
@@ -1394,7 +1394,7 @@
         <v>44191.5</v>
       </c>
       <c r="B87" t="n">
-        <v>430.5672302246094</v>
+        <v>372.0244140625</v>
       </c>
       <c r="C87" t="n">
         <v>341.1845370848899</v>
@@ -1405,7 +1405,7 @@
         <v>44191.54166666666</v>
       </c>
       <c r="B88" t="n">
-        <v>265.0321655273438</v>
+        <v>179.1565093994141</v>
       </c>
       <c r="C88" t="n">
         <v>135.5423672046378</v>
@@ -1416,7 +1416,7 @@
         <v>44191.58333333334</v>
       </c>
       <c r="B89" t="n">
-        <v>43.04627990722656</v>
+        <v>5.482924938201904</v>
       </c>
       <c r="C89" t="n">
         <v>0</v>
@@ -1427,7 +1427,7 @@
         <v>44191.625</v>
       </c>
       <c r="B90" t="n">
-        <v>22.68263244628906</v>
+        <v>21.53767395019531</v>
       </c>
       <c r="C90" t="n">
         <v>0</v>
@@ -1438,7 +1438,7 @@
         <v>44191.66666666666</v>
       </c>
       <c r="B91" t="n">
-        <v>14.87953090667725</v>
+        <v>-10.6082010269165</v>
       </c>
       <c r="C91" t="n">
         <v>0</v>
@@ -1449,7 +1449,7 @@
         <v>44191.70833333334</v>
       </c>
       <c r="B92" t="n">
-        <v>23.73829650878906</v>
+        <v>20.88002014160156</v>
       </c>
       <c r="C92" t="n">
         <v>0</v>
@@ -1460,7 +1460,7 @@
         <v>44191.75</v>
       </c>
       <c r="B93" t="n">
-        <v>13.752516746521</v>
+        <v>19.18049621582031</v>
       </c>
       <c r="C93" t="n">
         <v>0</v>
@@ -1471,7 +1471,7 @@
         <v>44191.79166666666</v>
       </c>
       <c r="B94" t="n">
-        <v>9.221877098083496</v>
+        <v>13.4560079574585</v>
       </c>
       <c r="C94" t="n">
         <v>0</v>
@@ -1482,7 +1482,7 @@
         <v>44191.83333333334</v>
       </c>
       <c r="B95" t="n">
-        <v>0.8817285895347595</v>
+        <v>10.5922384262085</v>
       </c>
       <c r="C95" t="n">
         <v>0</v>
@@ -1493,7 +1493,7 @@
         <v>44191.875</v>
       </c>
       <c r="B96" t="n">
-        <v>6.349441051483154</v>
+        <v>6.879592418670654</v>
       </c>
       <c r="C96" t="n">
         <v>0</v>
@@ -1504,7 +1504,7 @@
         <v>44191.91666666666</v>
       </c>
       <c r="B97" t="n">
-        <v>6.477797985076904</v>
+        <v>-9.354294776916504</v>
       </c>
       <c r="C97" t="n">
         <v>0</v>
@@ -1515,7 +1515,7 @@
         <v>44191.95833333334</v>
       </c>
       <c r="B98" t="n">
-        <v>7.860427379608154</v>
+        <v>-0.8933568596839905</v>
       </c>
       <c r="C98" t="n">
         <v>0</v>
@@ -1526,7 +1526,7 @@
         <v>44192</v>
       </c>
       <c r="B99" t="n">
-        <v>8.974867820739746</v>
+        <v>3.204421520233154</v>
       </c>
       <c r="C99" t="n">
         <v>0</v>
@@ -1537,7 +1537,7 @@
         <v>44192.04166666666</v>
       </c>
       <c r="B100" t="n">
-        <v>9.146437644958496</v>
+        <v>5.435378551483154</v>
       </c>
       <c r="C100" t="n">
         <v>0</v>
@@ -1548,7 +1548,7 @@
         <v>44192.08333333334</v>
       </c>
       <c r="B101" t="n">
-        <v>8.897902488708496</v>
+        <v>6.045058727264404</v>
       </c>
       <c r="C101" t="n">
         <v>0</v>
@@ -1559,7 +1559,7 @@
         <v>44192.125</v>
       </c>
       <c r="B102" t="n">
-        <v>9.414381980895996</v>
+        <v>5.735854625701904</v>
       </c>
       <c r="C102" t="n">
         <v>0</v>
@@ -1570,7 +1570,7 @@
         <v>44192.16666666666</v>
       </c>
       <c r="B103" t="n">
-        <v>11.700758934021</v>
+        <v>4.872695446014404</v>
       </c>
       <c r="C103" t="n">
         <v>0</v>
@@ -1581,7 +1581,7 @@
         <v>44192.20833333334</v>
       </c>
       <c r="B104" t="n">
-        <v>10.42787075042725</v>
+        <v>3.649611949920654</v>
       </c>
       <c r="C104" t="n">
         <v>0</v>
@@ -1592,7 +1592,7 @@
         <v>44192.25</v>
       </c>
       <c r="B105" t="n">
-        <v>23.92085266113281</v>
+        <v>50.92176818847656</v>
       </c>
       <c r="C105" t="n">
         <v>0</v>
@@ -1603,7 +1603,7 @@
         <v>44192.29166666666</v>
       </c>
       <c r="B106" t="n">
-        <v>404.0473937988281</v>
+        <v>516.832763671875</v>
       </c>
       <c r="C106" t="n">
         <v>508.6057987853231</v>
@@ -1614,7 +1614,7 @@
         <v>44192.33333333334</v>
       </c>
       <c r="B107" t="n">
-        <v>888.093994140625</v>
+        <v>835.8970336914062</v>
       </c>
       <c r="C107" t="n">
         <v>908.528543499407</v>
@@ -1625,7 +1625,7 @@
         <v>44192.375</v>
       </c>
       <c r="B108" t="n">
-        <v>1026.978759765625</v>
+        <v>909.7911376953125</v>
       </c>
       <c r="C108" t="n">
         <v>1082.138278033581</v>
@@ -1636,7 +1636,7 @@
         <v>44192.41666666666</v>
       </c>
       <c r="B109" t="n">
-        <v>1084.855224609375</v>
+        <v>894.4635620117188</v>
       </c>
       <c r="C109" t="n">
         <v>1117.777760599111</v>
@@ -1647,7 +1647,7 @@
         <v>44192.45833333334</v>
       </c>
       <c r="B110" t="n">
-        <v>625.9761962890625</v>
+        <v>489.2166748046875</v>
       </c>
       <c r="C110" t="n">
         <v>686.6762679260028</v>
@@ -1658,7 +1658,7 @@
         <v>44192.5</v>
       </c>
       <c r="B111" t="n">
-        <v>663.1019287109375</v>
+        <v>503.3908386230469</v>
       </c>
       <c r="C111" t="n">
         <v>650.9870009069275</v>
@@ -1669,7 +1669,7 @@
         <v>44192.54166666666</v>
       </c>
       <c r="B112" t="n">
-        <v>378.0867614746094</v>
+        <v>258.7674560546875</v>
       </c>
       <c r="C112" t="n">
         <v>304.3637426348992</v>
@@ -1680,7 +1680,7 @@
         <v>44192.58333333334</v>
       </c>
       <c r="B113" t="n">
-        <v>43.43287658691406</v>
+        <v>-57.88945007324219</v>
       </c>
       <c r="C113" t="n">
         <v>0</v>
@@ -1691,7 +1691,7 @@
         <v>44192.625</v>
       </c>
       <c r="B114" t="n">
-        <v>12.62782192230225</v>
+        <v>2.290847301483154</v>
       </c>
       <c r="C114" t="n">
         <v>0</v>
@@ -1702,7 +1702,7 @@
         <v>44192.66666666666</v>
       </c>
       <c r="B115" t="n">
-        <v>14.2584981918335</v>
+        <v>-46.90318298339844</v>
       </c>
       <c r="C115" t="n">
         <v>0</v>
@@ -1713,7 +1713,7 @@
         <v>44192.70833333334</v>
       </c>
       <c r="B116" t="n">
-        <v>20.35432434082031</v>
+        <v>10.11488246917725</v>
       </c>
       <c r="C116" t="n">
         <v>0</v>
@@ -1724,7 +1724,7 @@
         <v>44192.75</v>
       </c>
       <c r="B117" t="n">
-        <v>22.43287658691406</v>
+        <v>19.41151428222656</v>
       </c>
       <c r="C117" t="n">
         <v>0</v>
@@ -1735,7 +1735,7 @@
         <v>44192.79166666666</v>
       </c>
       <c r="B118" t="n">
-        <v>11.58546352386475</v>
+        <v>14.70558071136475</v>
       </c>
       <c r="C118" t="n">
         <v>0</v>
@@ -1746,7 +1746,7 @@
         <v>44192.83333333334</v>
       </c>
       <c r="B119" t="n">
-        <v>9.907729148864746</v>
+        <v>11.4235372543335</v>
       </c>
       <c r="C119" t="n">
         <v>0</v>
@@ -1757,7 +1757,7 @@
         <v>44192.875</v>
       </c>
       <c r="B120" t="n">
-        <v>8.523818016052246</v>
+        <v>7.706008434295654</v>
       </c>
       <c r="C120" t="n">
         <v>0</v>
@@ -1768,7 +1768,7 @@
         <v>44192.91666666666</v>
       </c>
       <c r="B121" t="n">
-        <v>13.6618185043335</v>
+        <v>-8.878769874572754</v>
       </c>
       <c r="C121" t="n">
         <v>0</v>
@@ -1779,7 +1779,7 @@
         <v>44192.95833333334</v>
       </c>
       <c r="B122" t="n">
-        <v>14.9225606918335</v>
+        <v>-1.605148911476135</v>
       </c>
       <c r="C122" t="n">
         <v>0</v>
@@ -1790,7 +1790,7 @@
         <v>44193</v>
       </c>
       <c r="B123" t="n">
-        <v>15.019850730896</v>
+        <v>2.217177867889404</v>
       </c>
       <c r="C123" t="n">
         <v>0</v>
@@ -1801,7 +1801,7 @@
         <v>44193.04166666666</v>
       </c>
       <c r="B124" t="n">
-        <v>13.665602684021</v>
+        <v>5.429458141326904</v>
       </c>
       <c r="C124" t="n">
         <v>0</v>
@@ -1812,7 +1812,7 @@
         <v>44193.08333333334</v>
       </c>
       <c r="B125" t="n">
-        <v>10.520827293396</v>
+        <v>6.798110485076904</v>
       </c>
       <c r="C125" t="n">
         <v>0</v>
@@ -1823,7 +1823,7 @@
         <v>44193.125</v>
       </c>
       <c r="B126" t="n">
-        <v>7.521987438201904</v>
+        <v>6.660903453826904</v>
       </c>
       <c r="C126" t="n">
         <v>0</v>
@@ -1834,7 +1834,7 @@
         <v>44193.16666666666</v>
       </c>
       <c r="B127" t="n">
-        <v>7.542373180389404</v>
+        <v>5.777602672576904</v>
       </c>
       <c r="C127" t="n">
         <v>0</v>
@@ -1845,7 +1845,7 @@
         <v>44193.20833333334</v>
       </c>
       <c r="B128" t="n">
-        <v>6.749465465545654</v>
+        <v>4.439773082733154</v>
       </c>
       <c r="C128" t="n">
         <v>0</v>
@@ -1856,7 +1856,7 @@
         <v>44193.25</v>
       </c>
       <c r="B129" t="n">
-        <v>5.185622692108154</v>
+        <v>16.79273986816406</v>
       </c>
       <c r="C129" t="n">
         <v>0</v>
@@ -1867,7 +1867,7 @@
         <v>44193.29166666666</v>
       </c>
       <c r="B130" t="n">
-        <v>162.8944244384766</v>
+        <v>229.2906036376953</v>
       </c>
       <c r="C130" t="n">
         <v>209.4137627790708</v>
@@ -1878,7 +1878,7 @@
         <v>44193.33333333334</v>
       </c>
       <c r="B131" t="n">
-        <v>800.2099609375</v>
+        <v>740.7918090820312</v>
       </c>
       <c r="C131" t="n">
         <v>816.5523276141247</v>
@@ -1889,7 +1889,7 @@
         <v>44193.375</v>
       </c>
       <c r="B132" t="n">
-        <v>747.2205200195312</v>
+        <v>687.0490112304688</v>
       </c>
       <c r="C132" t="n">
         <v>707.330723078645</v>
@@ -1900,7 +1900,7 @@
         <v>44193.41666666666</v>
       </c>
       <c r="B133" t="n">
-        <v>617.87646484375</v>
+        <v>448.335205078125</v>
       </c>
       <c r="C133" t="n">
         <v>583.5009192463716</v>
@@ -1911,7 +1911,7 @@
         <v>44193.45833333334</v>
       </c>
       <c r="B134" t="n">
-        <v>1067.919921875</v>
+        <v>933.514892578125</v>
       </c>
       <c r="C134" t="n">
         <v>1067.382617139933</v>
@@ -1922,7 +1922,7 @@
         <v>44193.5</v>
       </c>
       <c r="B135" t="n">
-        <v>839.5155029296875</v>
+        <v>603.0963745117188</v>
       </c>
       <c r="C135" t="n">
         <v>791.6446158832842</v>
@@ -1933,7 +1933,7 @@
         <v>44193.54166666666</v>
       </c>
       <c r="B136" t="n">
-        <v>399.0147705078125</v>
+        <v>280.5008850097656</v>
       </c>
       <c r="C136" t="n">
         <v>300.9817929880003</v>
@@ -1944,7 +1944,7 @@
         <v>44193.58333333334</v>
       </c>
       <c r="B137" t="n">
-        <v>28.24671936035156</v>
+        <v>-29.57676696777344</v>
       </c>
       <c r="C137" t="n">
         <v>0</v>
@@ -1955,7 +1955,7 @@
         <v>44193.625</v>
       </c>
       <c r="B138" t="n">
-        <v>13.3522481918335</v>
+        <v>10.09864711761475</v>
       </c>
       <c r="C138" t="n">
         <v>0</v>
@@ -1966,7 +1966,7 @@
         <v>44193.66666666666</v>
       </c>
       <c r="B139" t="n">
-        <v>22.44886779785156</v>
+        <v>-50.62858581542969</v>
       </c>
       <c r="C139" t="n">
         <v>0</v>
@@ -1977,7 +1977,7 @@
         <v>44193.70833333334</v>
       </c>
       <c r="B140" t="n">
-        <v>25.76319885253906</v>
+        <v>13.5541524887085</v>
       </c>
       <c r="C140" t="n">
         <v>0</v>
@@ -1988,7 +1988,7 @@
         <v>44193.75</v>
       </c>
       <c r="B141" t="n">
-        <v>17.29158020019531</v>
+        <v>18.93214416503906</v>
       </c>
       <c r="C141" t="n">
         <v>0</v>
@@ -1999,7 +1999,7 @@
         <v>44193.79166666666</v>
       </c>
       <c r="B142" t="n">
-        <v>15.74818325042725</v>
+        <v>11.11366176605225</v>
       </c>
       <c r="C142" t="n">
         <v>0</v>
@@ -2010,7 +2010,7 @@
         <v>44193.83333333334</v>
       </c>
       <c r="B143" t="n">
-        <v>10.56812953948975</v>
+        <v>9.700758934020996</v>
       </c>
       <c r="C143" t="n">
         <v>0</v>
@@ -2021,7 +2021,7 @@
         <v>44193.875</v>
       </c>
       <c r="B144" t="n">
-        <v>6.571547985076904</v>
+        <v>7.679885387420654</v>
       </c>
       <c r="C144" t="n">
         <v>0</v>
@@ -2032,7 +2032,7 @@
         <v>44193.91666666666</v>
       </c>
       <c r="B145" t="n">
-        <v>14.33924770355225</v>
+        <v>0.2220606058835983</v>
       </c>
       <c r="C145" t="n">
         <v>0</v>
@@ -2043,7 +2043,7 @@
         <v>44193.95833333334</v>
       </c>
       <c r="B146" t="n">
-        <v>14.28346157073975</v>
+        <v>5.197646617889404</v>
       </c>
       <c r="C146" t="n">
         <v>0</v>
@@ -2054,7 +2054,7 @@
         <v>44194</v>
       </c>
       <c r="B147" t="n">
-        <v>13.49098110198975</v>
+        <v>6.898574352264404</v>
       </c>
       <c r="C147" t="n">
         <v>0</v>
@@ -2065,7 +2065,7 @@
         <v>44194.04166666666</v>
       </c>
       <c r="B148" t="n">
-        <v>10.88136196136475</v>
+        <v>7.436233043670654</v>
       </c>
       <c r="C148" t="n">
         <v>0</v>
@@ -2076,7 +2076,7 @@
         <v>44194.08333333334</v>
       </c>
       <c r="B149" t="n">
-        <v>7.533889293670654</v>
+        <v>6.864638805389404</v>
       </c>
       <c r="C149" t="n">
         <v>0</v>
@@ -2087,7 +2087,7 @@
         <v>44194.125</v>
       </c>
       <c r="B150" t="n">
-        <v>3.611098766326904</v>
+        <v>5.358169078826904</v>
       </c>
       <c r="C150" t="n">
         <v>0</v>
@@ -2098,7 +2098,7 @@
         <v>44194.16666666666</v>
       </c>
       <c r="B151" t="n">
-        <v>0.4079126715660095</v>
+        <v>3.664199352264404</v>
       </c>
       <c r="C151" t="n">
         <v>0</v>
@@ -2109,7 +2109,7 @@
         <v>44194.20833333334</v>
       </c>
       <c r="B152" t="n">
-        <v>1.998427748680115</v>
+        <v>2.414077281951904</v>
       </c>
       <c r="C152" t="n">
         <v>0</v>
@@ -2120,7 +2120,7 @@
         <v>44194.25</v>
       </c>
       <c r="B153" t="n">
-        <v>29.93830871582031</v>
+        <v>49.30268859863281</v>
       </c>
       <c r="C153" t="n">
         <v>0</v>
@@ -2131,7 +2131,7 @@
         <v>44194.29166666666</v>
       </c>
       <c r="B154" t="n">
-        <v>441.8208923339844</v>
+        <v>513.603515625</v>
       </c>
       <c r="C154" t="n">
         <v>499.9815190426275</v>
@@ -2142,7 +2142,7 @@
         <v>44194.33333333334</v>
       </c>
       <c r="B155" t="n">
-        <v>831.5872192382812</v>
+        <v>777.1928100585938</v>
       </c>
       <c r="C155" t="n">
         <v>823.0417143182991</v>
@@ -2153,7 +2153,7 @@
         <v>44194.375</v>
       </c>
       <c r="B156" t="n">
-        <v>910.5470581054688</v>
+        <v>809.582763671875</v>
       </c>
       <c r="C156" t="n">
         <v>937.9135482272837</v>
@@ -2164,7 +2164,7 @@
         <v>44194.41666666666</v>
       </c>
       <c r="B157" t="n">
-        <v>1027.73583984375</v>
+        <v>874.2811889648438</v>
       </c>
       <c r="C157" t="n">
         <v>1055.477634523344</v>
@@ -2175,7 +2175,7 @@
         <v>44194.45833333334</v>
       </c>
       <c r="B158" t="n">
-        <v>1101.1171875</v>
+        <v>918.5062255859375</v>
       </c>
       <c r="C158" t="n">
         <v>1088.952196441093</v>
@@ -2186,7 +2186,7 @@
         <v>44194.5</v>
       </c>
       <c r="B159" t="n">
-        <v>582.6497802734375</v>
+        <v>454.0498046875</v>
       </c>
       <c r="C159" t="n">
         <v>597.3418299808457</v>
@@ -2197,7 +2197,7 @@
         <v>44194.54166666666</v>
       </c>
       <c r="B160" t="n">
-        <v>409.474853515625</v>
+        <v>240.6383819580078</v>
       </c>
       <c r="C160" t="n">
         <v>328.8786688740629</v>
@@ -2208,7 +2208,7 @@
         <v>44194.58333333334</v>
       </c>
       <c r="B161" t="n">
-        <v>42.42475891113281</v>
+        <v>-77.01066589355469</v>
       </c>
       <c r="C161" t="n">
         <v>0</v>
@@ -2219,7 +2219,7 @@
         <v>44194.625</v>
       </c>
       <c r="B162" t="n">
-        <v>11.9167013168335</v>
+        <v>-0.2181249409914017</v>
       </c>
       <c r="C162" t="n">
         <v>0</v>
@@ -2230,7 +2230,7 @@
         <v>44194.66666666666</v>
       </c>
       <c r="B163" t="n">
-        <v>16.98670959472656</v>
+        <v>-27.75267028808594</v>
       </c>
       <c r="C163" t="n">
         <v>0</v>
@@ -2241,7 +2241,7 @@
         <v>44194.70833333334</v>
       </c>
       <c r="B164" t="n">
-        <v>20.15150451660156</v>
+        <v>4.078139781951904</v>
       </c>
       <c r="C164" t="n">
         <v>0</v>
@@ -2252,7 +2252,7 @@
         <v>44194.75</v>
       </c>
       <c r="B165" t="n">
-        <v>16.84797668457031</v>
+        <v>16.22389221191406</v>
       </c>
       <c r="C165" t="n">
         <v>0</v>
@@ -2263,7 +2263,7 @@
         <v>44194.79166666666</v>
       </c>
       <c r="B166" t="n">
-        <v>14.438551902771</v>
+        <v>11.11878871917725</v>
       </c>
       <c r="C166" t="n">
         <v>0</v>
@@ -2274,7 +2274,7 @@
         <v>44194.83333333334</v>
       </c>
       <c r="B167" t="n">
-        <v>5.524978160858154</v>
+        <v>9.294264793395996</v>
       </c>
       <c r="C167" t="n">
         <v>0</v>
@@ -2285,7 +2285,7 @@
         <v>44194.875</v>
       </c>
       <c r="B168" t="n">
-        <v>6.561843395233154</v>
+        <v>7.386123180389404</v>
       </c>
       <c r="C168" t="n">
         <v>0</v>
@@ -2296,7 +2296,7 @@
         <v>44194.91666666666</v>
       </c>
       <c r="B169" t="n">
-        <v>12.8117208480835</v>
+        <v>7.204299449920654</v>
       </c>
       <c r="C169" t="n">
         <v>0</v>

</xml_diff>